<commit_message>
fix data latih data uji
</commit_message>
<xml_diff>
--- a/DATA TESTING & DATA UJI/datauji.xlsx
+++ b/DATA TESTING & DATA UJI/datauji.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\klasifikasi-data-tomat-metode-KNN\DATA TESTING &amp; DATA UJI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -331,7 +326,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B1" sqref="B1:H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>